<commit_message>
New Changes 12 7 dec
</commit_message>
<xml_diff>
--- a/SeleniumTests/TestData/Inputfile.xlsx
+++ b/SeleniumTests/TestData/Inputfile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="330" windowWidth="19815" windowHeight="2610"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="19815" windowHeight="6900"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -69,9 +70,6 @@
     <t>Accelerometer Test 2</t>
   </si>
   <si>
-    <t>Ser1122</t>
-  </si>
-  <si>
     <t>Repair Order</t>
   </si>
   <si>
@@ -84,9 +82,6 @@
     <t>Ship</t>
   </si>
   <si>
-    <t>Aut_123</t>
-  </si>
-  <si>
     <t>Kumar</t>
   </si>
   <si>
@@ -111,15 +106,9 @@
     <t>Ser2812</t>
   </si>
   <si>
-    <t>HW330278</t>
-  </si>
-  <si>
     <t>Aesthetic Check</t>
   </si>
   <si>
-    <t>PL546798</t>
-  </si>
-  <si>
     <t>TestOrd2811</t>
   </si>
   <si>
@@ -127,6 +116,18 @@
   </si>
   <si>
     <t>Test2134</t>
+  </si>
+  <si>
+    <t>Ord1272018</t>
+  </si>
+  <si>
+    <t>Ser1272018</t>
+  </si>
+  <si>
+    <t>HW117623</t>
+  </si>
+  <si>
+    <t>PL546711</t>
   </si>
 </sst>
 </file>
@@ -514,7 +515,7 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +545,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2">
         <v>43420</v>
@@ -586,7 +587,7 @@
         <v>6</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="P2" s="3">
         <v>1802401773</v>
@@ -601,14 +602,14 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>30</v>
+      <c r="A5" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -617,7 +618,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>14</v>
@@ -629,8 +630,8 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>30</v>
+      <c r="A7" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>14</v>
@@ -647,46 +648,46 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>30</v>
+      <c r="A9" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D9" s="3">
         <v>1802401773</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>30</v>
+      <c r="A11" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>14</v>
@@ -695,7 +696,7 @@
         <v>15</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -703,18 +704,18 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -723,21 +724,21 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>

</xml_diff>

<commit_message>
Due Date Cal Changes plus user directory changes
</commit_message>
<xml_diff>
--- a/SeleniumTests/TestData/Inputfile.xlsx
+++ b/SeleniumTests/TestData/Inputfile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="19815" windowHeight="6900"/>
+    <workbookView xWindow="0" yWindow="2565" windowWidth="19815" windowHeight="6780"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
   <si>
     <t>PO123</t>
   </si>
@@ -67,9 +66,6 @@
     <t>FAIL</t>
   </si>
   <si>
-    <t>Accelerometer Test 2</t>
-  </si>
-  <si>
     <t>Repair Order</t>
   </si>
   <si>
@@ -100,34 +96,91 @@
     <t>Test Unrepairable</t>
   </si>
   <si>
-    <t>Scrap</t>
-  </si>
-  <si>
-    <t>Ser2812</t>
-  </si>
-  <si>
     <t>Aesthetic Check</t>
   </si>
   <si>
-    <t>TestOrd2811</t>
-  </si>
-  <si>
     <t>External</t>
   </si>
   <si>
     <t>Test2134</t>
   </si>
   <si>
-    <t>Ord1272018</t>
-  </si>
-  <si>
-    <t>Ser1272018</t>
-  </si>
-  <si>
-    <t>HW117623</t>
-  </si>
-  <si>
-    <t>PL546711</t>
+    <t xml:space="preserve">Battery Status Test </t>
+  </si>
+  <si>
+    <t>Received</t>
+  </si>
+  <si>
+    <t>Repairable</t>
+  </si>
+  <si>
+    <t>Test1234</t>
+  </si>
+  <si>
+    <t>test123</t>
+  </si>
+  <si>
+    <t>Create Part</t>
+  </si>
+  <si>
+    <t>TestDescription</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Component Picking</t>
+  </si>
+  <si>
+    <t>Component Putaway</t>
+  </si>
+  <si>
+    <t>Repair And Replace</t>
+  </si>
+  <si>
+    <t>Ravi1234</t>
+  </si>
+  <si>
+    <t>Part Picking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C01A01 </t>
+  </si>
+  <si>
+    <t>Deliver Part</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>Printer</t>
+  </si>
+  <si>
+    <t>Replaced</t>
+  </si>
+  <si>
+    <t>Ser12562018</t>
+  </si>
+  <si>
+    <t>DueDateCalc</t>
+  </si>
+  <si>
+    <t>Ord12182018</t>
+  </si>
+  <si>
+    <t>Ser12182018</t>
+  </si>
+  <si>
+    <t>PN536744</t>
+  </si>
+  <si>
+    <t>HWNB6531</t>
+  </si>
+  <si>
+    <t>MX7T160926876</t>
+  </si>
+  <si>
+    <t>HWPN1234</t>
   </si>
 </sst>
 </file>
@@ -159,7 +212,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -195,11 +248,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -211,6 +275,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,18 +578,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
@@ -533,19 +599,21 @@
     <col min="12" max="12" width="15.42578125" customWidth="1"/>
     <col min="13" max="13" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" customWidth="1"/>
+    <col min="15" max="15" width="13" customWidth="1"/>
     <col min="16" max="16" width="12.28515625" customWidth="1"/>
     <col min="17" max="17" width="12.7109375" customWidth="1"/>
+    <col min="18" max="18" width="21.5703125" customWidth="1"/>
+    <col min="19" max="19" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="B2" s="2">
         <v>43420</v>
@@ -587,29 +655,35 @@
         <v>6</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P2" s="3">
-        <v>1802401773</v>
+        <v>50</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -618,20 +692,20 @@
         <v>12</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>14</v>
@@ -640,110 +714,217 @@
         <v>15</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1802401773</v>
+        <v>31</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J9" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>28</v>
+        <v>49</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1300</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1090</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>200381676</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="2">
+        <v>43420</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Create Branch and User Repository
</commit_message>
<xml_diff>
--- a/SeleniumTests/TestData/Inputfile.xlsx
+++ b/SeleniumTests/TestData/Inputfile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2565" windowWidth="19815" windowHeight="6780"/>
+    <workbookView xWindow="0" yWindow="2625" windowWidth="19815" windowHeight="6720"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="73">
   <si>
     <t>PO123</t>
   </si>
@@ -199,6 +199,42 @@
   </si>
   <si>
     <t>Dateline Standard Time</t>
+  </si>
+  <si>
+    <t>BranchMaster</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>TestUser</t>
+  </si>
+  <si>
+    <t>Address1</t>
+  </si>
+  <si>
+    <t>Address line 2</t>
+  </si>
+  <si>
+    <t>TestCity</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Contact Name</t>
+  </si>
+  <si>
+    <t>Contact Phone</t>
+  </si>
+  <si>
+    <t>Contact Email</t>
   </si>
 </sst>
 </file>
@@ -588,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S29"/>
+  <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,10 +638,11 @@
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="30.42578125" customWidth="1"/>
-    <col min="9" max="10" width="16.5703125" customWidth="1"/>
-    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.28515625" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" customWidth="1"/>
     <col min="12" max="12" width="15.42578125" customWidth="1"/>
     <col min="13" max="13" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -840,7 +877,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>40</v>
       </c>
@@ -860,12 +897,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>42</v>
       </c>
@@ -876,12 +913,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
@@ -892,12 +929,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>33</v>
       </c>
@@ -908,24 +945,24 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>200381675</v>
       </c>
@@ -939,12 +976,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>59</v>
       </c>
@@ -953,6 +990,49 @@
       </c>
       <c r="C29" s="1" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TestData from excel for BranchMaster and UserMaster
</commit_message>
<xml_diff>
--- a/SeleniumTests/TestData/Inputfile.xlsx
+++ b/SeleniumTests/TestData/Inputfile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2625" windowWidth="19815" windowHeight="6720"/>
+    <workbookView xWindow="0" yWindow="2685" windowWidth="19815" windowHeight="6660"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="80">
   <si>
     <t>PO123</t>
   </si>
@@ -207,34 +207,55 @@
     <t>New York</t>
   </si>
   <si>
-    <t>TestUser</t>
-  </si>
-  <si>
-    <t>Address1</t>
-  </si>
-  <si>
     <t>Address line 2</t>
   </si>
   <si>
     <t>TestCity</t>
   </si>
   <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Zip</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
     <t>Contact Name</t>
   </si>
   <si>
-    <t>Contact Phone</t>
-  </si>
-  <si>
-    <t>Contact Email</t>
+    <t>USerMaster</t>
+  </si>
+  <si>
+    <t>TestBranch</t>
+  </si>
+  <si>
+    <t>TestAdd</t>
+  </si>
+  <si>
+    <t>TestState</t>
+  </si>
+  <si>
+    <t>TestZip</t>
+  </si>
+  <si>
+    <t>TestCountry</t>
+  </si>
+  <si>
+    <t>Test@ctdi.com</t>
+  </si>
+  <si>
+    <t>BinsMaster</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Tuser</t>
+  </si>
+  <si>
+    <t>Tuser@gmail.com</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>ViewOrders</t>
   </si>
 </sst>
 </file>
@@ -624,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="A33" sqref="A33:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,42 +1023,79 @@
         <v>62</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="F31" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>58</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
+      </c>
+      <c r="K31" s="1">
+        <v>9999999999</v>
       </c>
       <c r="L31" s="1" t="s">
         <v>72</v>
       </c>
     </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L31" r:id="rId1"/>
+    <hyperlink ref="D33" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated scripts to capture new UI changes
</commit_message>
<xml_diff>
--- a/SeleniumTests/TestData/Inputfile.xlsx
+++ b/SeleniumTests/TestData/Inputfile.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="88">
   <si>
     <t>PO123</t>
   </si>
@@ -78,15 +78,6 @@
     <t>Ship</t>
   </si>
   <si>
-    <t>Kumar</t>
-  </si>
-  <si>
-    <t>Intermittent Power</t>
-  </si>
-  <si>
-    <t>Damaged Component</t>
-  </si>
-  <si>
     <t>Test Repairable</t>
   </si>
   <si>
@@ -153,9 +144,6 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>Replaced</t>
-  </si>
-  <si>
     <t>DueDateCalc</t>
   </si>
   <si>
@@ -168,27 +156,12 @@
     <t xml:space="preserve">PartsPicking </t>
   </si>
   <si>
-    <t>PP536744</t>
-  </si>
-  <si>
     <t>Ord12992018</t>
   </si>
   <si>
     <t>Ser12992018</t>
   </si>
   <si>
-    <t>PB536744</t>
-  </si>
-  <si>
-    <t>Non-conforming bin</t>
-  </si>
-  <si>
-    <t>HWSN1531</t>
-  </si>
-  <si>
-    <t>Ser11</t>
-  </si>
-  <si>
     <t>Manage Region</t>
   </si>
   <si>
@@ -265,6 +238,48 @@
   </si>
   <si>
     <t>EditDescription</t>
+  </si>
+  <si>
+    <t>TestPrinter</t>
+  </si>
+  <si>
+    <t>TestBin</t>
+  </si>
+  <si>
+    <t>SN00006</t>
+  </si>
+  <si>
+    <t>ZBSN1880</t>
+  </si>
+  <si>
+    <t>Battery-Diminished</t>
+  </si>
+  <si>
+    <t>Battery Tray</t>
+  </si>
+  <si>
+    <t>REPLACE/INSTALL</t>
+  </si>
+  <si>
+    <t>SN00009</t>
+  </si>
+  <si>
+    <t>AH00001</t>
+  </si>
+  <si>
+    <t>Pack878899</t>
+  </si>
+  <si>
+    <t>AG00001</t>
+  </si>
+  <si>
+    <t>FEDEX</t>
+  </si>
+  <si>
+    <t>STANDARD OVERNIGHT</t>
+  </si>
+  <si>
+    <t>USD</t>
   </si>
 </sst>
 </file>
@@ -659,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,8 +685,7 @@
     <col min="3" max="3" width="23.140625" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" customWidth="1"/>
+    <col min="6" max="7" width="22.28515625" customWidth="1"/>
     <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.28515625" customWidth="1"/>
     <col min="10" max="10" width="16.5703125" customWidth="1"/>
@@ -693,7 +707,7 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2">
         <v>43420</v>
@@ -735,19 +749,19 @@
         <v>6</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -757,13 +771,13 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -772,13 +786,13 @@
         <v>12</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -788,19 +802,19 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -810,34 +824,37 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="J9" s="6" t="s">
-        <v>45</v>
+        <v>80</v>
+      </c>
+      <c r="K9" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -847,16 +864,16 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -869,13 +886,13 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -889,74 +906,82 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C17" s="1">
         <v>1300</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E17" s="1">
         <v>1090</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>14</v>
@@ -964,35 +989,35 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1000,128 +1025,128 @@
         <v>200381675</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C27" s="2">
         <v>43420</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="I31" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="K31" s="1">
         <v>9999999999</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D35" s="3">
         <v>1373</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F35" s="3">
         <v>12</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>